<commit_message>
Finish Random Numbers Generator
</commit_message>
<xml_diff>
--- a/Quantitative-Methods/RandomNumbers/random_numbers.xlsx
+++ b/Quantitative-Methods/RandomNumbers/random_numbers.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Desktop\Cuantitativos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data-Science\Quantitative-Methods\RandomNumbers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA4BC63-79A5-4F9A-8F35-D286BD58E4FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED125B62-2B85-4222-B147-523DF5DCE519}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13550" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A76358BE-4536-40ED-8A37-B64FE8E79E32}"/>
   </bookViews>
   <sheets>
     <sheet name="random" sheetId="1" r:id="rId1"/>
+    <sheet name="histogram" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>m</t>
   </si>
@@ -53,15 +54,52 @@
   <si>
     <t>xi</t>
   </si>
+  <si>
+    <t>TRUNC</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>MAX</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>SUB_W</t>
+  </si>
+  <si>
+    <t>DECIMALS</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Lower Limit</t>
+  </si>
+  <si>
+    <t>Upper limit</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000000000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,17 +116,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF212121"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF212121"/>
-      <name val="Arial"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -100,7 +133,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FF9900CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -134,16 +167,18 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -196,13 +231,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Classes</a:t>
+              <a:t>Histogram</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs. Frequency</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Random Numbers</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -257,40 +296,40 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>random!$L$3:$L$10</c:f>
+              <c:f>histogram!$H$3:$H$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7.6679999999999998E-2</c:v>
+                  <c:v>7.6550000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19808100000000001</c:v>
+                  <c:v>0.19795000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31948199999999999</c:v>
+                  <c:v>0.31935000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.44088300000000002</c:v>
+                  <c:v>0.44074999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.56228400000000001</c:v>
+                  <c:v>0.56214999999999993</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.68368499999999999</c:v>
+                  <c:v>0.68354999999999988</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.80508599999999997</c:v>
+                  <c:v>0.80494999999999983</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.92648699999999995</c:v>
+                  <c:v>0.92639999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>random!$M$3:$M$10</c:f>
+              <c:f>histogram!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -323,7 +362,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8CFE-4A8B-B398-B84BE5DAE6C9}"/>
+              <c16:uniqueId val="{00000000-98CA-418C-996C-E623423B2F83}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -337,71 +376,16 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="921326912"/>
-        <c:axId val="921328160"/>
+        <c:axId val="1028391615"/>
+        <c:axId val="1028394111"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="921326912"/>
+        <c:axId val="1028391615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Classes</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -439,7 +423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="921328160"/>
+        <c:crossAx val="1028394111"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -447,7 +431,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="921328160"/>
+        <c:axId val="1028394111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,61 +451,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Frequency</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -553,7 +482,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="921326912"/>
+        <c:crossAx val="1028391615"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1149,23 +1078,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>203653</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>94796</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>525991</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>64028</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>508453</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>170996</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>10582</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>140228</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20B952EE-6559-4EA1-9983-EC0AA198CBB5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40F60686-D71C-4376-B6E3-4D14AB3BC12E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1483,19 +1412,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54ECAA78-C9A7-4060-8C0C-544F66893B5D}">
-  <dimension ref="A1:M101"/>
+  <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1514,8 +1444,11 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2147483647</v>
       </c>
@@ -1536,9 +1469,12 @@
         <f>E2/$A$2</f>
         <v>0.96622006966090768</v>
       </c>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G2" s="1">
+        <f>TRUNC(F2,histogram!B$4)</f>
+        <v>0.96619999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3">
         <f>MOD(E2*$B$2+$C$2,$A$2)</f>
         <v>559872160</v>
@@ -1547,25 +1483,12 @@
         <f>E3/$A$2</f>
         <v>0.26071079087476751</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5">
-        <v>1.5980000000000001E-2</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0.13738</v>
-      </c>
-      <c r="L3" s="5">
-        <v>7.6679999999999998E-2</v>
-      </c>
-      <c r="M3" s="6">
-        <f>COUNTIFS($F$2:$F$2000,"&lt;="&amp;K3,$F$2:$F$2000,"&gt;="&amp;J3)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G3" s="1">
+        <f>TRUNC(F3,histogram!B$4)</f>
+        <v>0.26069999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E4">
         <f t="shared" ref="E4:E67" si="0">MOD(E3*$B$2+$C$2,$A$2)</f>
         <v>1645535613</v>
@@ -1574,25 +1497,12 @@
         <f t="shared" ref="F4:F67" si="1">E4/$A$2</f>
         <v>0.76626223221712852</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5">
-        <v>2</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.137381</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0.25878099999999998</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0.19808100000000001</v>
-      </c>
-      <c r="M4" s="6">
-        <f>COUNTIFS($F$2:$F$2000,"&lt;="&amp;K4,$F$2:$F$2000,"&gt;="&amp;J4)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <f>TRUNC(F4,histogram!B$4)</f>
+        <v>0.76619999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5">
         <f t="shared" si="0"/>
         <v>1222641625</v>
@@ -1601,25 +1511,12 @@
         <f t="shared" si="1"/>
         <v>0.56933687327864435</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5">
-        <v>3</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0.25878200000000001</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0.38018200000000002</v>
-      </c>
-      <c r="L5" s="5">
-        <v>0.31948199999999999</v>
-      </c>
-      <c r="M5" s="6">
-        <f>COUNTIFS($F$2:$F$2000,"&lt;="&amp;K5,$F$2:$F$2000,"&gt;="&amp;J5)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <f>TRUNC(F5,histogram!B$4)</f>
+        <v>0.56930000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6">
         <f t="shared" si="0"/>
         <v>1814256879</v>
@@ -1628,25 +1525,12 @@
         <f t="shared" si="1"/>
         <v>0.84482919417546554</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="5">
-        <v>4</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.38018299999999999</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0.501583</v>
-      </c>
-      <c r="L6" s="5">
-        <v>0.44088300000000002</v>
-      </c>
-      <c r="M6" s="6">
-        <f>COUNTIFS($F$2:$F$2000,"&lt;="&amp;K6,$F$2:$F$2000,"&gt;="&amp;J6)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <f>TRUNC(F6,histogram!B$4)</f>
+        <v>0.8448</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7">
         <f t="shared" si="0"/>
         <v>95061600</v>
@@ -1655,25 +1539,12 @@
         <f t="shared" si="1"/>
         <v>4.4266507050146585E-2</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="5">
-        <v>5</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0.50158400000000003</v>
-      </c>
-      <c r="K7" s="5">
-        <v>0.62298399999999998</v>
-      </c>
-      <c r="L7" s="5">
-        <v>0.56228400000000001</v>
-      </c>
-      <c r="M7" s="6">
-        <f>COUNTIFS($F$2:$F$2000,"&lt;="&amp;K7,$F$2:$F$2000,"&gt;="&amp;J7)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G7" s="1">
+        <f>TRUNC(F7,histogram!B$4)</f>
+        <v>4.4200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E8">
         <f t="shared" si="0"/>
         <v>2119961479</v>
@@ -1682,25 +1553,12 @@
         <f t="shared" si="1"/>
         <v>0.98718399181365224</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="5">
-        <v>6</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0.62298500000000001</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0.74438499999999996</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0.68368499999999999</v>
-      </c>
-      <c r="M8" s="6">
-        <f>COUNTIFS($F$2:$F$2000,"&lt;="&amp;K8,$F$2:$F$2000,"&gt;="&amp;J8)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G8" s="1">
+        <f>TRUNC(F8,histogram!B$4)</f>
+        <v>0.98709999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E9">
         <f t="shared" si="0"/>
         <v>1291390176</v>
@@ -1709,25 +1567,12 @@
         <f t="shared" si="1"/>
         <v>0.60135041205275352</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="5">
-        <v>7</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0.74438599999999999</v>
-      </c>
-      <c r="K9" s="5">
-        <v>0.86578599999999994</v>
-      </c>
-      <c r="L9" s="5">
-        <v>0.80508599999999997</v>
-      </c>
-      <c r="M9" s="6">
-        <f>COUNTIFS($F$2:$F$2000,"&lt;="&amp;K9,$F$2:$F$2000,"&gt;="&amp;J9)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G9" s="1">
+        <f>TRUNC(F9,histogram!B$4)</f>
+        <v>0.60129999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10">
         <f t="shared" si="0"/>
         <v>1924951450</v>
@@ -1736,25 +1581,12 @@
         <f t="shared" si="1"/>
         <v>0.89637537062930661</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="5">
-        <v>8</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0.86578699999999997</v>
-      </c>
-      <c r="K10" s="5">
-        <v>0.98718700000000004</v>
-      </c>
-      <c r="L10" s="5">
-        <v>0.92648699999999995</v>
-      </c>
-      <c r="M10" s="6">
-        <f>COUNTIFS($F$2:$F$2000,"&lt;="&amp;K10,$F$2:$F$2000,"&gt;="&amp;J10)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G10" s="1">
+        <f>TRUNC(F10,histogram!B$4)</f>
+        <v>0.89629999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E11">
         <f t="shared" si="0"/>
         <v>817878095</v>
@@ -1763,9 +1595,12 @@
         <f t="shared" si="1"/>
         <v>0.38085416675585049</v>
       </c>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <f>TRUNC(F11,histogram!B$4)</f>
+        <v>0.38080000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E12">
         <f t="shared" si="0"/>
         <v>34318218</v>
@@ -1774,9 +1609,12 @@
         <f t="shared" si="1"/>
         <v>1.5980665579429208E-2</v>
       </c>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <f>TRUNC(F12,histogram!B$4)</f>
+        <v>1.5900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13">
         <f t="shared" si="0"/>
         <v>1260672530</v>
@@ -1785,12 +1623,12 @@
         <f t="shared" si="1"/>
         <v>0.58704639346666931</v>
       </c>
-      <c r="M13">
-        <f>SUM(M3:M10)</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <f>TRUNC(F13,histogram!B$4)</f>
+        <v>0.58699999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14">
         <f t="shared" si="0"/>
         <v>1049550408</v>
@@ -1799,8 +1637,12 @@
         <f t="shared" si="1"/>
         <v>0.48873499431122791</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G14" s="1">
+        <f>TRUNC(F14,histogram!B$4)</f>
+        <v>0.48870000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E15">
         <f t="shared" si="0"/>
         <v>363030798</v>
@@ -1809,8 +1651,12 @@
         <f t="shared" si="1"/>
         <v>0.16904938880775561</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <f>TRUNC(F15,histogram!B$4)</f>
+        <v>0.16900000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E16">
         <f t="shared" si="0"/>
         <v>457580859</v>
@@ -1819,8 +1665,12 @@
         <f t="shared" si="1"/>
         <v>0.21307769194854315</v>
       </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1">
+        <f>TRUNC(F16,histogram!B$4)</f>
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E17">
         <f t="shared" si="0"/>
         <v>422557306</v>
@@ -1829,8 +1679,12 @@
         <f t="shared" si="1"/>
         <v>0.1967685791648778</v>
       </c>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1">
+        <f>TRUNC(F17,histogram!B$4)</f>
+        <v>0.19670000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E18">
         <f t="shared" si="0"/>
         <v>192221313</v>
@@ -1839,8 +1693,12 @@
         <f t="shared" si="1"/>
         <v>8.9510024101245228E-2</v>
       </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1">
+        <f>TRUNC(F18,histogram!B$4)</f>
+        <v>8.9499999999999996E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E19">
         <f t="shared" si="0"/>
         <v>848202503</v>
@@ -1849,8 +1707,12 @@
         <f t="shared" si="1"/>
         <v>0.39497506962855117</v>
       </c>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="1">
+        <f>TRUNC(F19,histogram!B$4)</f>
+        <v>0.39489999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E20">
         <f t="shared" si="0"/>
         <v>743019135</v>
@@ -1859,8 +1721,12 @@
         <f t="shared" si="1"/>
         <v>0.34599524705949947</v>
       </c>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1">
+        <f>TRUNC(F20,histogram!B$4)</f>
+        <v>0.34589999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E21">
         <f t="shared" si="0"/>
         <v>305194640</v>
@@ -1869,8 +1735,12 @@
         <f t="shared" si="1"/>
         <v>0.14211732900800059</v>
       </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1">
+        <f>TRUNC(F21,histogram!B$4)</f>
+        <v>0.1421</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E22">
         <f t="shared" si="0"/>
         <v>1215365444</v>
@@ -1879,8 +1749,12 @@
         <f t="shared" si="1"/>
         <v>0.5659486374659225</v>
       </c>
-    </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="1">
+        <f>TRUNC(F22,histogram!B$4)</f>
+        <v>0.56589999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E23">
         <f t="shared" si="0"/>
         <v>1930050691</v>
@@ -1889,8 +1763,12 @@
         <f t="shared" si="1"/>
         <v>0.89874988975876469</v>
       </c>
-    </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="1">
+        <f>TRUNC(F23,histogram!B$4)</f>
+        <v>0.89870000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E24">
         <f t="shared" si="0"/>
         <v>621475702</v>
@@ -1899,8 +1777,12 @@
         <f t="shared" si="1"/>
         <v>0.28939717555856198</v>
       </c>
-    </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="1">
+        <f>TRUNC(F24,histogram!B$4)</f>
+        <v>0.2893</v>
+      </c>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E25">
         <f t="shared" si="0"/>
         <v>1929148153</v>
@@ -1909,8 +1791,12 @@
         <f t="shared" si="1"/>
         <v>0.8983296127516448</v>
       </c>
-    </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="1">
+        <f>TRUNC(F25,histogram!B$4)</f>
+        <v>0.89829999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E26">
         <f t="shared" si="0"/>
         <v>484905065</v>
@@ -1919,8 +1805,12 @@
         <f t="shared" si="1"/>
         <v>0.22580151689509001</v>
       </c>
-    </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="1">
+        <f>TRUNC(F26,histogram!B$4)</f>
+        <v>0.2258</v>
+      </c>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E27">
         <f t="shared" si="0"/>
         <v>98987090</v>
@@ -1929,8 +1819,12 @@
         <f t="shared" si="1"/>
         <v>4.609445577771145E-2</v>
       </c>
-    </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="1">
+        <f>TRUNC(F27,histogram!B$4)</f>
+        <v>4.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E28">
         <f t="shared" si="0"/>
         <v>1523678852</v>
@@ -1939,8 +1833,12 @@
         <f t="shared" si="1"/>
         <v>0.70951825599629348</v>
       </c>
-    </row>
-    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="1">
+        <f>TRUNC(F28,histogram!B$4)</f>
+        <v>0.70950000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E29">
         <f t="shared" si="0"/>
         <v>1875458736</v>
@@ -1949,8 +1847,12 @@
         <f t="shared" si="1"/>
         <v>0.87332852970498076</v>
       </c>
-    </row>
-    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="1">
+        <f>TRUNC(F29,histogram!B$4)</f>
+        <v>0.87329999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E30">
         <f t="shared" si="0"/>
         <v>70005286</v>
@@ -1959,8 +1861,12 @@
         <f t="shared" si="1"/>
         <v>3.2598751612286432E-2</v>
       </c>
-    </row>
-    <row r="31" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="1">
+        <f>TRUNC(F30,histogram!B$4)</f>
+        <v>3.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E31">
         <f t="shared" si="0"/>
         <v>1905286893</v>
@@ -1969,8 +1875,12 @@
         <f t="shared" si="1"/>
         <v>0.88721834769808605</v>
       </c>
-    </row>
-    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="1">
+        <f>TRUNC(F31,histogram!B$4)</f>
+        <v>0.88719999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E32">
         <f t="shared" si="0"/>
         <v>1028150234</v>
@@ -1979,8 +1889,12 @@
         <f t="shared" si="1"/>
         <v>0.4787697617331379</v>
       </c>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="1">
+        <f>TRUNC(F32,histogram!B$4)</f>
+        <v>0.47870000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E33">
         <f t="shared" si="0"/>
         <v>1467559076</v>
@@ -1989,8 +1903,12 @@
         <f t="shared" si="1"/>
         <v>0.68338544884854246</v>
       </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="1">
+        <f>TRUNC(F33,histogram!B$4)</f>
+        <v>0.68330000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E34">
         <f t="shared" si="0"/>
         <v>1415704537</v>
@@ -1999,8 +1917,12 @@
         <f t="shared" si="1"/>
         <v>0.65923879745380898</v>
       </c>
-    </row>
-    <row r="35" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="1">
+        <f>TRUNC(F34,histogram!B$4)</f>
+        <v>0.65920000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E35">
         <f t="shared" si="0"/>
         <v>1774828246</v>
@@ -2009,8 +1931,12 @@
         <f t="shared" si="1"/>
         <v>0.82646880616735141</v>
       </c>
-    </row>
-    <row r="36" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="1">
+        <f>TRUNC(F35,histogram!B$4)</f>
+        <v>0.82640000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E36">
         <f t="shared" si="0"/>
         <v>990473692</v>
@@ -2019,8 +1945,12 @@
         <f t="shared" si="1"/>
         <v>0.461225254675944</v>
       </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="1">
+        <f>TRUNC(F36,histogram!B$4)</f>
+        <v>0.4612</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E37">
         <f t="shared" si="0"/>
         <v>1745593547</v>
@@ -2029,8 +1959,12 @@
         <f t="shared" si="1"/>
         <v>0.81285533859061787</v>
       </c>
-    </row>
-    <row r="38" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="1">
+        <f>TRUNC(F37,histogram!B$4)</f>
+        <v>0.81279999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E38">
         <f t="shared" si="0"/>
         <v>1416642762</v>
@@ -2039,8 +1973,12 @@
         <f t="shared" si="1"/>
         <v>0.65967569251529667</v>
       </c>
-    </row>
-    <row r="39" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="1">
+        <f>TRUNC(F38,histogram!B$4)</f>
+        <v>0.65959999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E39">
         <f t="shared" si="0"/>
         <v>363706645</v>
@@ -2049,8 +1987,12 @@
         <f t="shared" si="1"/>
         <v>0.16936410459194523</v>
       </c>
-    </row>
-    <row r="40" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="1">
+        <f>TRUNC(F39,histogram!B$4)</f>
+        <v>0.16930000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E40">
         <f t="shared" si="0"/>
         <v>1079123153</v>
@@ -2059,8 +2001,12 @@
         <f t="shared" si="1"/>
         <v>0.50250587682356396</v>
       </c>
-    </row>
-    <row r="41" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="1">
+        <f>TRUNC(F40,histogram!B$4)</f>
+        <v>0.50249999999999995</v>
+      </c>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E41">
         <f t="shared" si="0"/>
         <v>1323433556</v>
@@ -2069,8 +2015,12 @@
         <f t="shared" si="1"/>
         <v>0.61627177364019292</v>
       </c>
-    </row>
-    <row r="42" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="1">
+        <f>TRUNC(F41,histogram!B$4)</f>
+        <v>0.61619999999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E42">
         <f t="shared" si="0"/>
         <v>1459643713</v>
@@ -2079,8 +2029,12 @@
         <f t="shared" si="1"/>
         <v>0.67969957072273812</v>
       </c>
-    </row>
-    <row r="43" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="1">
+        <f>TRUNC(F42,histogram!B$4)</f>
+        <v>0.67959999999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E43">
         <f t="shared" si="0"/>
         <v>1526184710</v>
@@ -2089,8 +2043,12 @@
         <f t="shared" si="1"/>
         <v>0.71068513705892733</v>
       </c>
-    </row>
-    <row r="44" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="1">
+        <f>TRUNC(F43,histogram!B$4)</f>
+        <v>0.71060000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E44">
         <f t="shared" si="0"/>
         <v>1041741202</v>
@@ -2099,8 +2057,12 @@
         <f t="shared" si="1"/>
         <v>0.48509854939072328</v>
       </c>
-    </row>
-    <row r="45" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="1">
+        <f>TRUNC(F44,histogram!B$4)</f>
+        <v>0.48499999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E45">
         <f t="shared" si="0"/>
         <v>110208023</v>
@@ -2109,8 +2071,12 @@
         <f t="shared" si="1"/>
         <v>5.1319609885718494E-2</v>
       </c>
-    </row>
-    <row r="46" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="1">
+        <f>TRUNC(F45,histogram!B$4)</f>
+        <v>5.1299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E46">
         <f t="shared" si="0"/>
         <v>1135338847</v>
@@ -2119,8 +2085,12 @@
         <f t="shared" si="1"/>
         <v>0.52868334927069183</v>
       </c>
-    </row>
-    <row r="47" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="1">
+        <f>TRUNC(F46,histogram!B$4)</f>
+        <v>0.52859999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E47">
         <f t="shared" si="0"/>
         <v>1247797934</v>
@@ -2129,8 +2099,12 @@
         <f t="shared" si="1"/>
         <v>0.58105119251695048</v>
       </c>
-    </row>
-    <row r="48" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="1">
+        <f>TRUNC(F47,histogram!B$4)</f>
+        <v>0.58099999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E48">
         <f t="shared" si="0"/>
         <v>1562063783</v>
@@ -2139,8 +2113,12 @@
         <f t="shared" si="1"/>
         <v>0.72739263238729568</v>
       </c>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="1">
+        <f>TRUNC(F48,histogram!B$4)</f>
+        <v>0.72729999999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E49">
         <f t="shared" si="0"/>
         <v>618416306</v>
@@ -2149,8 +2127,12 @@
         <f t="shared" si="1"/>
         <v>0.28797253327815447</v>
       </c>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="1">
+        <f>TRUNC(F49,histogram!B$4)</f>
+        <v>0.28789999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E50">
         <f t="shared" si="0"/>
         <v>2049487109</v>
@@ -2159,8 +2141,12 @@
         <f t="shared" si="1"/>
         <v>0.95436680594196865</v>
       </c>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="1">
+        <f>TRUNC(F50,histogram!B$4)</f>
+        <v>0.95430000000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E51">
         <f t="shared" si="0"/>
         <v>92143083</v>
@@ -2169,8 +2155,12 @@
         <f t="shared" si="1"/>
         <v>4.2907466666264209E-2</v>
       </c>
-    </row>
-    <row r="52" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="1">
+        <f>TRUNC(F51,histogram!B$4)</f>
+        <v>4.2900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E52">
         <f t="shared" si="0"/>
         <v>313086494</v>
@@ -2179,8 +2169,12 @@
         <f t="shared" si="1"/>
         <v>0.14579225990259659</v>
       </c>
-    </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="1">
+        <f>TRUNC(F52,histogram!B$4)</f>
+        <v>0.1457</v>
+      </c>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E53">
         <f t="shared" si="0"/>
         <v>709769508</v>
@@ -2189,8 +2183,12 @@
         <f t="shared" si="1"/>
         <v>0.33051218294096746</v>
       </c>
-    </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="1">
+        <f>TRUNC(F53,histogram!B$4)</f>
+        <v>0.33050000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54">
         <f t="shared" si="0"/>
         <v>1971945518</v>
@@ -2199,8 +2197,12 @@
         <f t="shared" si="1"/>
         <v>0.91825868884020423</v>
       </c>
-    </row>
-    <row r="55" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="1">
+        <f>TRUNC(F54,histogram!B$4)</f>
+        <v>0.91820000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E55">
         <f t="shared" si="0"/>
         <v>373196875</v>
@@ -2209,8 +2211,12 @@
         <f t="shared" si="1"/>
         <v>0.17378333731264964</v>
       </c>
-    </row>
-    <row r="56" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="1">
+        <f>TRUNC(F55,histogram!B$4)</f>
+        <v>0.17369999999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E56">
         <f t="shared" si="0"/>
         <v>1667628885</v>
@@ -2219,8 +2225,12 @@
         <f t="shared" si="1"/>
         <v>0.77655021370227928</v>
       </c>
-    </row>
-    <row r="57" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="1">
+        <f>TRUNC(F56,histogram!B$4)</f>
+        <v>0.77649999999999997</v>
+      </c>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E57">
         <f t="shared" si="0"/>
         <v>1029593198</v>
@@ -2229,8 +2239,12 @@
         <f t="shared" si="1"/>
         <v>0.47944169420722949</v>
       </c>
-    </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="1">
+        <f>TRUNC(F57,histogram!B$4)</f>
+        <v>0.47939999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E58">
         <f t="shared" si="0"/>
         <v>2097134907</v>
@@ -2239,8 +2253,12 @@
         <f t="shared" si="1"/>
         <v>0.97655454090635974</v>
       </c>
-    </row>
-    <row r="59" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="1">
+        <f>TRUNC(F58,histogram!B$4)</f>
+        <v>0.97650000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E59">
         <f t="shared" si="0"/>
         <v>2044767385</v>
@@ -2249,8 +2267,12 @@
         <f t="shared" si="1"/>
         <v>0.95216901318736791</v>
       </c>
-    </row>
-    <row r="60" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="1">
+        <f>TRUNC(F59,histogram!B$4)</f>
+        <v>0.95209999999999995</v>
+      </c>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E60">
         <f t="shared" si="0"/>
         <v>224636754</v>
@@ -2259,8 +2281,12 @@
         <f t="shared" si="1"/>
         <v>0.10460464009298227</v>
       </c>
-    </row>
-    <row r="61" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="1">
+        <f>TRUNC(F60,histogram!B$4)</f>
+        <v>0.1046</v>
+      </c>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E61">
         <f t="shared" si="0"/>
         <v>193673052</v>
@@ -2269,8 +2295,12 @@
         <f t="shared" si="1"/>
         <v>9.0186042753134868E-2</v>
       </c>
-    </row>
-    <row r="62" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="1">
+        <f>TRUNC(F61,histogram!B$4)</f>
+        <v>9.01E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E62">
         <f t="shared" si="0"/>
         <v>1625259759</v>
@@ -2279,8 +2309,12 @@
         <f t="shared" si="1"/>
         <v>0.75682055193782805</v>
       </c>
-    </row>
-    <row r="63" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="1">
+        <f>TRUNC(F62,histogram!B$4)</f>
+        <v>0.75680000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E63">
         <f t="shared" si="0"/>
         <v>1896263320</v>
@@ -2289,8 +2323,12 @@
         <f t="shared" si="1"/>
         <v>0.88301641907683404</v>
       </c>
-    </row>
-    <row r="64" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="1">
+        <f>TRUNC(F63,histogram!B$4)</f>
+        <v>0.88300000000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E64">
         <f t="shared" si="0"/>
         <v>1840297760</v>
@@ -2299,8 +2337,12 @@
         <f t="shared" si="1"/>
         <v>0.8569554243502</v>
       </c>
-    </row>
-    <row r="65" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G64" s="1">
+        <f>TRUNC(F64,histogram!B$4)</f>
+        <v>0.8569</v>
+      </c>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E65">
         <f t="shared" si="0"/>
         <v>1824968226</v>
@@ -2309,8 +2351,12 @@
         <f t="shared" si="1"/>
         <v>0.84981705381060813</v>
       </c>
-    </row>
-    <row r="66" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G65" s="1">
+        <f>TRUNC(F65,histogram!B$4)</f>
+        <v>0.8498</v>
+      </c>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E66">
         <f t="shared" si="0"/>
         <v>1879527928</v>
@@ -2319,8 +2365,12 @@
         <f t="shared" si="1"/>
         <v>0.87522339489088552</v>
       </c>
-    </row>
-    <row r="67" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G66" s="1">
+        <f>TRUNC(F66,histogram!B$4)</f>
+        <v>0.87519999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E67">
         <f t="shared" si="0"/>
         <v>1888922173</v>
@@ -2329,8 +2379,12 @@
         <f t="shared" si="1"/>
         <v>0.87959793111290685</v>
       </c>
-    </row>
-    <row r="68" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G67" s="1">
+        <f>TRUNC(F67,histogram!B$4)</f>
+        <v>0.87949999999999995</v>
+      </c>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E68">
         <f t="shared" ref="E68:E101" si="2">MOD(E67*$B$2+$C$2,$A$2)</f>
         <v>864208010</v>
@@ -2339,8 +2393,12 @@
         <f t="shared" ref="F68:F101" si="3">E68/$A$2</f>
         <v>0.40242821462565487</v>
       </c>
-    </row>
-    <row r="69" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G68" s="1">
+        <f>TRUNC(F68,histogram!B$4)</f>
+        <v>0.40239999999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E69">
         <f t="shared" si="2"/>
         <v>1312119409</v>
@@ -2349,8 +2407,12 @@
         <f t="shared" si="3"/>
         <v>0.61100321338093055</v>
       </c>
-    </row>
-    <row r="70" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G69" s="1">
+        <f>TRUNC(F69,histogram!B$4)</f>
+        <v>0.61099999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E70">
         <f t="shared" si="2"/>
         <v>281336020</v>
@@ -2359,8 +2421,12 @@
         <f t="shared" si="3"/>
         <v>0.13100729330024091</v>
       </c>
-    </row>
-    <row r="71" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G70" s="1">
+        <f>TRUNC(F70,histogram!B$4)</f>
+        <v>0.13100000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E71">
         <f t="shared" si="2"/>
         <v>1802981093</v>
@@ -2369,8 +2435,12 @@
         <f t="shared" si="3"/>
         <v>0.83957849714885391</v>
       </c>
-    </row>
-    <row r="72" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G71" s="1">
+        <f>TRUNC(F71,histogram!B$4)</f>
+        <v>0.83950000000000002</v>
+      </c>
+    </row>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E72">
         <f t="shared" si="2"/>
         <v>1708970881</v>
@@ -2379,8 +2449,12 @@
         <f t="shared" si="3"/>
         <v>0.79580158078847529</v>
       </c>
-    </row>
-    <row r="73" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G72" s="1">
+        <f>TRUNC(F72,histogram!B$4)</f>
+        <v>0.79579999999999995</v>
+      </c>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E73">
         <f t="shared" si="2"/>
         <v>79818342</v>
@@ -2389,8 +2463,12 @@
         <f t="shared" si="3"/>
         <v>3.7168311903797234E-2</v>
       </c>
-    </row>
-    <row r="74" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G73" s="1">
+        <f>TRUNC(F73,histogram!B$4)</f>
+        <v>3.7100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E74">
         <f t="shared" si="2"/>
         <v>1477078266</v>
@@ -2399,8 +2477,12 @@
         <f t="shared" si="3"/>
         <v>0.68781816712013355</v>
       </c>
-    </row>
-    <row r="75" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G74" s="1">
+        <f>TRUNC(F74,histogram!B$4)</f>
+        <v>0.68779999999999997</v>
+      </c>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E75">
         <f t="shared" si="2"/>
         <v>343457342</v>
@@ -2409,8 +2491,12 @@
         <f t="shared" si="3"/>
         <v>0.15993478808548989</v>
       </c>
-    </row>
-    <row r="76" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G75" s="1">
+        <f>TRUNC(F75,histogram!B$4)</f>
+        <v>0.15989999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E76">
         <f t="shared" si="2"/>
         <v>51503858</v>
@@ -2419,8 +2505,12 @@
         <f t="shared" si="3"/>
         <v>2.3983352828763124E-2</v>
       </c>
-    </row>
-    <row r="77" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G76" s="1">
+        <f>TRUNC(F76,histogram!B$4)</f>
+        <v>2.3900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E77">
         <f t="shared" si="2"/>
         <v>189431665</v>
@@ -2429,8 +2519,12 @@
         <f t="shared" si="3"/>
         <v>8.8210993021824863E-2</v>
       </c>
-    </row>
-    <row r="78" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G77" s="1">
+        <f>TRUNC(F77,histogram!B$4)</f>
+        <v>8.8200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E78">
         <f t="shared" si="2"/>
         <v>1207228801</v>
@@ -2439,8 +2533,12 @@
         <f t="shared" si="3"/>
         <v>0.56215971781041463</v>
       </c>
-    </row>
-    <row r="79" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G78" s="1">
+        <f>TRUNC(F78,histogram!B$4)</f>
+        <v>0.56210000000000004</v>
+      </c>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E79">
         <f t="shared" si="2"/>
         <v>468961551</v>
@@ -2449,8 +2547,12 @@
         <f t="shared" si="3"/>
         <v>0.21837723963818384</v>
       </c>
-    </row>
-    <row r="80" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G79" s="1">
+        <f>TRUNC(F79,histogram!B$4)</f>
+        <v>0.21829999999999999</v>
+      </c>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E80">
         <f t="shared" si="2"/>
         <v>571803167</v>
@@ -2459,8 +2561,12 @@
         <f t="shared" si="3"/>
         <v>0.26626659895585225</v>
       </c>
-    </row>
-    <row r="81" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G80" s="1">
+        <f>TRUNC(F80,histogram!B$4)</f>
+        <v>0.26619999999999999</v>
+      </c>
+    </row>
+    <row r="81" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E81">
         <f t="shared" si="2"/>
         <v>306507444</v>
@@ -2469,8 +2575,12 @@
         <f t="shared" si="3"/>
         <v>0.142728651008908</v>
       </c>
-    </row>
-    <row r="82" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G81" s="1">
+        <f>TRUNC(F81,histogram!B$4)</f>
+        <v>0.14269999999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E82">
         <f t="shared" si="2"/>
         <v>1804825802</v>
@@ -2479,8 +2589,12 @@
         <f t="shared" si="3"/>
         <v>0.84043750671690209</v>
       </c>
-    </row>
-    <row r="83" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G82" s="1">
+        <f>TRUNC(F82,histogram!B$4)</f>
+        <v>0.84040000000000004</v>
+      </c>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E83">
         <f t="shared" si="2"/>
         <v>500740339</v>
@@ -2489,8 +2603,12 @@
         <f t="shared" si="3"/>
         <v>0.23317539097423451</v>
       </c>
-    </row>
-    <row r="84" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G83" s="1">
+        <f>TRUNC(F83,histogram!B$4)</f>
+        <v>0.2331</v>
+      </c>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E84">
         <f t="shared" si="2"/>
         <v>2101948627</v>
@@ -2499,8 +2617,12 @@
         <f t="shared" si="3"/>
         <v>0.97879610395934247</v>
       </c>
-    </row>
-    <row r="85" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G84" s="1">
+        <f>TRUNC(F84,histogram!B$4)</f>
+        <v>0.97870000000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E85">
         <f t="shared" si="2"/>
         <v>1344580839</v>
@@ -2509,8 +2631,12 @@
         <f t="shared" si="3"/>
         <v>0.62611924466961955</v>
       </c>
-    </row>
-    <row r="86" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G85" s="1">
+        <f>TRUNC(F85,histogram!B$4)</f>
+        <v>0.62609999999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E86">
         <f t="shared" si="2"/>
         <v>399743692</v>
@@ -2519,8 +2645,12 @@
         <f t="shared" si="3"/>
         <v>0.18614516229654904</v>
       </c>
-    </row>
-    <row r="87" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G86" s="1">
+        <f>TRUNC(F86,histogram!B$4)</f>
+        <v>0.18609999999999999</v>
+      </c>
+    </row>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E87">
         <f t="shared" si="2"/>
         <v>1163383628</v>
@@ -2529,8 +2659,12 @@
         <f t="shared" si="3"/>
         <v>0.5417427180994967</v>
       </c>
-    </row>
-    <row r="88" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G87" s="1">
+        <f>TRUNC(F87,histogram!B$4)</f>
+        <v>0.54169999999999996</v>
+      </c>
+    </row>
+    <row r="88" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E88">
         <f t="shared" si="2"/>
         <v>150029861</v>
@@ -2539,8 +2673,12 @@
         <f t="shared" si="3"/>
         <v>6.9863098240393731E-2</v>
       </c>
-    </row>
-    <row r="89" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G88" s="1">
+        <f>TRUNC(F88,histogram!B$4)</f>
+        <v>6.9800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E89">
         <f t="shared" si="2"/>
         <v>406072249</v>
@@ -2549,8 +2687,12 @@
         <f t="shared" si="3"/>
         <v>0.18909212629734171</v>
       </c>
-    </row>
-    <row r="90" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G89" s="1">
+        <f>TRUNC(F89,histogram!B$4)</f>
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="90" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E90">
         <f t="shared" si="2"/>
         <v>153258777</v>
@@ -2559,8 +2701,12 @@
         <f t="shared" si="3"/>
         <v>7.1366679422262436E-2</v>
       </c>
-    </row>
-    <row r="91" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G90" s="1">
+        <f>TRUNC(F90,histogram!B$4)</f>
+        <v>7.1300000000000002E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E91">
         <f t="shared" si="2"/>
         <v>987372286</v>
@@ -2569,8 +2715,12 @@
         <f t="shared" si="3"/>
         <v>0.45978104996484753</v>
       </c>
-    </row>
-    <row r="92" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G91" s="1">
+        <f>TRUNC(F91,histogram!B$4)</f>
+        <v>0.4597</v>
+      </c>
+    </row>
+    <row r="92" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E92">
         <f t="shared" si="2"/>
         <v>1159870433</v>
@@ -2579,8 +2729,12 @@
         <f t="shared" si="3"/>
         <v>0.54010675919247175</v>
       </c>
-    </row>
-    <row r="93" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G92" s="1">
+        <f>TRUNC(F92,histogram!B$4)</f>
+        <v>0.54010000000000002</v>
+      </c>
+    </row>
+    <row r="93" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E93">
         <f t="shared" si="2"/>
         <v>1233303612</v>
@@ -2589,8 +2743,12 @@
         <f t="shared" si="3"/>
         <v>0.57430174787263466</v>
       </c>
-    </row>
-    <row r="94" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G93" s="1">
+        <f>TRUNC(F93,histogram!B$4)</f>
+        <v>0.57430000000000003</v>
+      </c>
+    </row>
+    <row r="94" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E94">
         <f t="shared" si="2"/>
         <v>621646040</v>
@@ -2599,8 +2757,12 @@
         <f t="shared" si="3"/>
         <v>0.28947649537095638</v>
       </c>
-    </row>
-    <row r="95" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G94" s="1">
+        <f>TRUNC(F94,histogram!B$4)</f>
+        <v>0.28939999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E95">
         <f t="shared" si="2"/>
         <v>497051625</v>
@@ -2609,8 +2771,12 @@
         <f t="shared" si="3"/>
         <v>0.23145769966368457</v>
       </c>
-    </row>
-    <row r="96" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G95" s="1">
+        <f>TRUNC(F95,histogram!B$4)</f>
+        <v>0.23139999999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E96">
         <f t="shared" si="2"/>
         <v>235274545</v>
@@ -2619,8 +2785,12 @@
         <f t="shared" si="3"/>
         <v>0.10955824754645967</v>
       </c>
-    </row>
-    <row r="97" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G96" s="1">
+        <f>TRUNC(F96,histogram!B$4)</f>
+        <v>0.1095</v>
+      </c>
+    </row>
+    <row r="97" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E97">
         <f t="shared" si="2"/>
         <v>741883688</v>
@@ -2629,8 +2799,12 @@
         <f t="shared" si="3"/>
         <v>0.34546651334756356</v>
       </c>
-    </row>
-    <row r="98" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G97" s="1">
+        <f>TRUNC(F97,histogram!B$4)</f>
+        <v>0.34539999999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E98">
         <f t="shared" si="2"/>
         <v>549089734</v>
@@ -2639,8 +2813,12 @@
         <f t="shared" si="3"/>
         <v>0.25568983250096899</v>
       </c>
-    </row>
-    <row r="99" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G98" s="1">
+        <f>TRUNC(F98,histogram!B$4)</f>
+        <v>0.25559999999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E99">
         <f t="shared" si="2"/>
         <v>813928179</v>
@@ -2649,8 +2827,12 @@
         <f t="shared" si="3"/>
         <v>0.37901484378567657</v>
       </c>
-    </row>
-    <row r="100" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G99" s="1">
+        <f>TRUNC(F99,histogram!B$4)</f>
+        <v>0.379</v>
+      </c>
+    </row>
+    <row r="100" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E100">
         <f t="shared" si="2"/>
         <v>220073063</v>
@@ -2659,8 +2841,12 @@
         <f t="shared" si="3"/>
         <v>0.10247950586605795</v>
       </c>
-    </row>
-    <row r="101" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="G100" s="1">
+        <f>TRUNC(F100,histogram!B$4)</f>
+        <v>0.1024</v>
+      </c>
+    </row>
+    <row r="101" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E101">
         <f t="shared" si="2"/>
         <v>801129707</v>
@@ -2668,11 +2854,293 @@
       <c r="F101" s="1">
         <f t="shared" si="3"/>
         <v>0.37305509083580929</v>
+      </c>
+      <c r="G101" s="1">
+        <f>TRUNC(F101,histogram!B$4)</f>
+        <v>0.373</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0455BE2A-39F5-4152-9A3E-E87F5D196DC0}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1">
+        <f>COUNT(random!G2:G101)</f>
+        <v>100</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <f>MAX(random!G2:G101)</f>
+        <v>0.98709999999999998</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <f>MIN(random!G2:G101)</f>
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <f>B3</f>
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="G3" s="6">
+        <f>F4-$B$7</f>
+        <v>0.13720000000000002</v>
+      </c>
+      <c r="H3" s="5">
+        <f>AVERAGE(F3:G3)</f>
+        <v>7.6550000000000007E-2</v>
+      </c>
+      <c r="I3" s="5">
+        <f>COUNTIFS(random!G$2:G$101,"&lt;="&amp;G3,random!G$2:G$101,"&gt;="&amp;F3)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <f>F3+$B$6</f>
+        <v>0.13730000000000001</v>
+      </c>
+      <c r="G4" s="6">
+        <f>G3+$B$6</f>
+        <v>0.2586</v>
+      </c>
+      <c r="H4" s="5">
+        <f>AVERAGE(F4:G4)</f>
+        <v>0.19795000000000001</v>
+      </c>
+      <c r="I4" s="5">
+        <f>COUNTIFS(random!G$2:G$101,"&lt;="&amp;G4,random!G$2:G$101,"&gt;="&amp;F4)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <f>1+3.3*LOG10(B1)</f>
+        <v>7.6</v>
+      </c>
+      <c r="C5">
+        <f>ROUNDUP(B5,0)</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6">
+        <f t="shared" ref="F5:F11" si="0">F4+$B$6</f>
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" ref="G5:G11" si="1">G4+$B$6</f>
+        <v>0.38</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" ref="H4:H11" si="2">AVERAGE(F5:G5)</f>
+        <v>0.31935000000000002</v>
+      </c>
+      <c r="I5" s="5">
+        <f>COUNTIFS(random!G$2:G$101,"&lt;="&amp;G5,random!G$2:G$101,"&gt;="&amp;F5)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <f>ROUNDUP((B2-B3)/C5,B4)</f>
+        <v>0.12139999999999999</v>
+      </c>
+      <c r="E6" s="5">
+        <v>4</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.38009999999999999</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="1"/>
+        <v>0.50139999999999996</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="2"/>
+        <v>0.44074999999999998</v>
+      </c>
+      <c r="I6" s="5">
+        <f>COUNTIFS(random!G$2:G$101,"&lt;="&amp;G6,random!G$2:G$101,"&gt;="&amp;F6)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <f>1/10^B4</f>
+        <v>1E-4</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5</v>
+      </c>
+      <c r="F7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.50149999999999995</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.62279999999999991</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="2"/>
+        <v>0.56214999999999993</v>
+      </c>
+      <c r="I7" s="5">
+        <f>COUNTIFS(random!G$2:G$101,"&lt;="&amp;G7,random!G$2:G$101,"&gt;="&amp;F7)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8" s="5">
+        <v>6</v>
+      </c>
+      <c r="F8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.6228999999999999</v>
+      </c>
+      <c r="G8" s="6">
+        <f t="shared" si="1"/>
+        <v>0.74419999999999986</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="2"/>
+        <v>0.68354999999999988</v>
+      </c>
+      <c r="I8" s="5">
+        <f>COUNTIFS(random!G$2:G$101,"&lt;="&amp;G8,random!G$2:G$101,"&gt;="&amp;F8)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="5">
+        <v>7</v>
+      </c>
+      <c r="F9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.74429999999999985</v>
+      </c>
+      <c r="G9" s="6">
+        <f t="shared" si="1"/>
+        <v>0.86559999999999981</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="2"/>
+        <v>0.80494999999999983</v>
+      </c>
+      <c r="I9" s="5">
+        <f>COUNTIFS(random!G$2:G$101,"&lt;="&amp;G9,random!G$2:G$101,"&gt;="&amp;F9)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="5">
+        <v>8</v>
+      </c>
+      <c r="F10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8656999999999998</v>
+      </c>
+      <c r="G10" s="6">
+        <f>B2</f>
+        <v>0.98709999999999998</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="2"/>
+        <v>0.92639999999999989</v>
+      </c>
+      <c r="I10" s="5">
+        <f>COUNTIFS(random!G$2:G$101,"&lt;="&amp;G10,random!G$2:G$101,"&gt;="&amp;F10)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f>SUM(I3:I10)</f>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>